<commit_message>
Updated vegas scraper and scores scraper
</commit_message>
<xml_diff>
--- a/backend/data/analytics/3_consecutive_scores.xlsx
+++ b/backend/data/analytics/3_consecutive_scores.xlsx
@@ -7,10 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Percentages" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Counts" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Season Percentages" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Season Counts" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10 Year Percentages" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10 Year Counts" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5 Year Percentages" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5 Year Counts" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Season Percentages" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Season Counts" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,450 +441,416 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>total</t>
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B2" t="n">
         <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>56.99999999999999</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>62</v>
-      </c>
-      <c r="H2" t="n">
-        <v>71</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D3" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>60</v>
-      </c>
-      <c r="H3" t="n">
-        <v>56.00000000000001</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C4" t="n">
         <v>52</v>
       </c>
       <c r="D4" t="n">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E4" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F4" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G4" t="n">
-        <v>67</v>
-      </c>
-      <c r="H4" t="n">
-        <v>65</v>
-      </c>
-      <c r="I4" t="n">
-        <v>50</v>
-      </c>
-      <c r="J4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C5" t="n">
-        <v>56.99999999999999</v>
+        <v>64</v>
       </c>
       <c r="D5" t="n">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E5" t="n">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F5" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G5" t="n">
-        <v>69</v>
-      </c>
-      <c r="H5" t="n">
-        <v>78</v>
-      </c>
-      <c r="I5" t="n">
-        <v>100</v>
-      </c>
-      <c r="J5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C6" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D6" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" t="n">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G6" t="n">
-        <v>60</v>
-      </c>
-      <c r="H6" t="n">
-        <v>67</v>
-      </c>
-      <c r="I6" t="n">
-        <v>100</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="C7" t="n">
+        <v>64</v>
+      </c>
+      <c r="D7" t="n">
+        <v>64</v>
+      </c>
+      <c r="E7" t="n">
+        <v>70</v>
+      </c>
+      <c r="F7" t="n">
         <v>60</v>
       </c>
-      <c r="D7" t="n">
-        <v>73</v>
-      </c>
-      <c r="E7" t="n">
-        <v>65</v>
-      </c>
-      <c r="F7" t="n">
-        <v>76</v>
-      </c>
       <c r="G7" t="n">
-        <v>45</v>
-      </c>
-      <c r="H7" t="n">
-        <v>70</v>
-      </c>
-      <c r="I7" t="n">
-        <v>100</v>
-      </c>
-      <c r="J7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C8" t="n">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D8" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E8" t="n">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F8" t="n">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="G8" t="n">
         <v>83</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>100</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C9" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D9" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E9" t="n">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F9" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G9" t="n">
-        <v>100</v>
-      </c>
-      <c r="H9" t="n">
         <v>67</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>57.99999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D10" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E10" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F10" t="n">
-        <v>55.00000000000001</v>
+        <v>56.99999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>50</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F11" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="E12" t="n">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="F12" t="n">
         <v>100</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="F13" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G14" t="n">
-        <v>100</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>60</v>
+      </c>
+      <c r="D15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>100</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -897,7 +865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,450 +876,416 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>total</t>
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
-      </c>
-      <c r="H2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>148</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>35</v>
-      </c>
-      <c r="H3" t="n">
-        <v>16</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D4" t="n">
-        <v>253</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>341</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
-        <v>316</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>123</v>
-      </c>
-      <c r="H4" t="n">
-        <v>54</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D5" t="n">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="E5" t="n">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="F5" t="n">
-        <v>127</v>
+        <v>8</v>
       </c>
       <c r="G5" t="n">
-        <v>36</v>
-      </c>
-      <c r="H5" t="n">
-        <v>18</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B6" t="n">
+        <v>43</v>
+      </c>
+      <c r="C6" t="n">
+        <v>176</v>
+      </c>
+      <c r="D6" t="n">
+        <v>96</v>
+      </c>
+      <c r="E6" t="n">
+        <v>32</v>
+      </c>
+      <c r="F6" t="n">
+        <v>18</v>
+      </c>
+      <c r="G6" t="n">
         <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>13</v>
-      </c>
-      <c r="D6" t="n">
-        <v>101</v>
-      </c>
-      <c r="E6" t="n">
-        <v>171</v>
-      </c>
-      <c r="F6" t="n">
-        <v>159</v>
-      </c>
-      <c r="G6" t="n">
-        <v>60</v>
-      </c>
-      <c r="H6" t="n">
-        <v>21</v>
-      </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B7" t="n">
+        <v>33</v>
+      </c>
+      <c r="C7" t="n">
+        <v>137</v>
+      </c>
+      <c r="D7" t="n">
+        <v>87</v>
+      </c>
+      <c r="E7" t="n">
+        <v>37</v>
+      </c>
+      <c r="F7" t="n">
+        <v>15</v>
+      </c>
+      <c r="G7" t="n">
         <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>37</v>
-      </c>
-      <c r="E7" t="n">
-        <v>57</v>
-      </c>
-      <c r="F7" t="n">
-        <v>59</v>
-      </c>
-      <c r="G7" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" t="n">
-        <v>10</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>310</v>
       </c>
       <c r="D8" t="n">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="E8" t="n">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="F8" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G8" t="n">
         <v>6</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="D9" t="n">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="E9" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" t="n">
-        <v>8</v>
-      </c>
-      <c r="H9" t="n">
         <v>3</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>229</v>
       </c>
       <c r="D10" t="n">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="F10" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" t="n">
         <v>1</v>
-      </c>
-      <c r="F12" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" t="n">
         <v>1</v>
       </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1361,6 +1295,784 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" t="n">
+        <v>71</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B4" t="n">
+        <v>63</v>
+      </c>
+      <c r="C4" t="n">
+        <v>51</v>
+      </c>
+      <c r="D4" t="n">
+        <v>55.00000000000001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>80</v>
+      </c>
+      <c r="F4" t="n">
+        <v>33</v>
+      </c>
+      <c r="G4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B5" t="n">
+        <v>56.00000000000001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>66</v>
+      </c>
+      <c r="D5" t="n">
+        <v>64</v>
+      </c>
+      <c r="E5" t="n">
+        <v>83</v>
+      </c>
+      <c r="F5" t="n">
+        <v>62</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>60</v>
+      </c>
+      <c r="C6" t="n">
+        <v>59</v>
+      </c>
+      <c r="D6" t="n">
+        <v>67</v>
+      </c>
+      <c r="E6" t="n">
+        <v>67</v>
+      </c>
+      <c r="F6" t="n">
+        <v>83</v>
+      </c>
+      <c r="G6" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B7" t="n">
+        <v>44</v>
+      </c>
+      <c r="C7" t="n">
+        <v>62</v>
+      </c>
+      <c r="D7" t="n">
+        <v>55.00000000000001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>81</v>
+      </c>
+      <c r="F7" t="n">
+        <v>60</v>
+      </c>
+      <c r="G7" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B8" t="n">
+        <v>62</v>
+      </c>
+      <c r="C8" t="n">
+        <v>65</v>
+      </c>
+      <c r="D8" t="n">
+        <v>64</v>
+      </c>
+      <c r="E8" t="n">
+        <v>60</v>
+      </c>
+      <c r="F8" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" t="n">
+        <v>57.99999999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>62</v>
+      </c>
+      <c r="E9" t="n">
+        <v>76</v>
+      </c>
+      <c r="F9" t="n">
+        <v>60</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B10" t="n">
+        <v>50</v>
+      </c>
+      <c r="C10" t="n">
+        <v>65</v>
+      </c>
+      <c r="D10" t="n">
+        <v>73</v>
+      </c>
+      <c r="E10" t="n">
+        <v>47</v>
+      </c>
+      <c r="F10" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B11" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" t="n">
+        <v>67</v>
+      </c>
+      <c r="D11" t="n">
+        <v>67</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>67</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B12" t="n">
+        <v>75</v>
+      </c>
+      <c r="C12" t="n">
+        <v>53</v>
+      </c>
+      <c r="D12" t="n">
+        <v>64</v>
+      </c>
+      <c r="E12" t="n">
+        <v>60</v>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>67</v>
+      </c>
+      <c r="D13" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>50</v>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>100</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>17</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n">
+        <v>70</v>
+      </c>
+      <c r="D4" t="n">
+        <v>42</v>
+      </c>
+      <c r="E4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>67</v>
+      </c>
+      <c r="D5" t="n">
+        <v>42</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C6" t="n">
+        <v>125</v>
+      </c>
+      <c r="D6" t="n">
+        <v>107</v>
+      </c>
+      <c r="E6" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" t="n">
+        <v>23</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B7" t="n">
+        <v>18</v>
+      </c>
+      <c r="C7" t="n">
+        <v>87</v>
+      </c>
+      <c r="D7" t="n">
+        <v>51</v>
+      </c>
+      <c r="E7" t="n">
+        <v>27</v>
+      </c>
+      <c r="F7" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B8" t="n">
+        <v>42</v>
+      </c>
+      <c r="C8" t="n">
+        <v>124</v>
+      </c>
+      <c r="D8" t="n">
+        <v>91</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35</v>
+      </c>
+      <c r="F8" t="n">
+        <v>21</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>43</v>
+      </c>
+      <c r="D9" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" t="n">
+        <v>17</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>30</v>
+      </c>
+      <c r="E10" t="n">
+        <v>19</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>36</v>
+      </c>
+      <c r="D11" t="n">
+        <v>18</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>19</v>
+      </c>
+      <c r="D12" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1377,37 +2089,37 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>total</t>
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>25</v>
@@ -1424,22 +2136,22 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D3" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1447,45 +2159,45 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B4" t="n">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C4" t="n">
-        <v>56.99999999999999</v>
+        <v>64</v>
       </c>
       <c r="D4" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E4" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F4" t="n">
         <v>50</v>
       </c>
       <c r="G4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B5" t="n">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C5" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D5" t="n">
-        <v>56.99999999999999</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1493,45 +2205,45 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C6" t="n">
-        <v>70</v>
+        <v>56.99999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1539,7 +2251,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B8" t="n">
         <v>100</v>
@@ -1548,13 +2260,13 @@
         <v>80</v>
       </c>
       <c r="D8" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E8" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1562,16 +2274,16 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1585,16 +2297,16 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D10" t="n">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1608,16 +2320,16 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1634,7 +2346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1651,46 +2363,46 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>total</t>
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -1698,22 +2410,22 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
         <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1721,45 +2433,45 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" t="n">
         <v>9</v>
       </c>
-      <c r="C4" t="n">
-        <v>21</v>
-      </c>
-      <c r="D4" t="n">
-        <v>22</v>
-      </c>
-      <c r="E4" t="n">
-        <v>15</v>
-      </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B5" t="n">
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1767,45 +2479,45 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" t="n">
         <v>2</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1813,22 +2525,22 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1836,16 +2548,16 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1859,19 +2571,19 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1882,16 +2594,16 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>

</xml_diff>